<commit_message>
Added two break beam sensors, one with a 5mm beam and one with a 3mm beam. A 5mm beam is a bit more robust and that might be important since there most likely will be some collision with other robots.
</commit_message>
<xml_diff>
--- a/BOM/RoboCUP_SSL_Hardware_BOM.xlsx
+++ b/BOM/RoboCUP_SSL_Hardware_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fnl18001\OneDrive - Mälardalens universitet\Robotics_program_university\Ongoing_courses\DVA490\SSL-Hardware-Development\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_746B6E28CE293E4F3E464F6686B02C4FF617E8F7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{26BAEA5D-5913-4A8E-B3D9-228D25EF71D5}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_746B6E28CE293E4F3E464F6686B02C4FF617E8F7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3CD2EEE0-48D2-4CF5-B9D2-A2FB5DC246C8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,40 +29,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Unknown Author</author>
-  </authors>
-  <commentList>
-    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Fredrik Westerbom:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Haven't reveived a quotation so I cannot know the price.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="40">
   <si>
     <t>Communication Component</t>
   </si>
@@ -167,13 +135,28 @@
   </si>
   <si>
     <t>7,9*8,8*0,8</t>
+  </si>
+  <si>
+    <t>IR Break Beam Sensors with Premium Wire Header Ends - 3mm LEDs</t>
+  </si>
+  <si>
+    <t>IR Break Beam Sensors with Premium Wire Header Ends - 3mm LEDs : ID 2167 : Adafruit Industries, Unique &amp; fun DIY electronics and kits</t>
+  </si>
+  <si>
+    <t>(20*10*8)</t>
+  </si>
+  <si>
+    <t>IR Break Beam Sensor with Premium Wire Header Ends - 5mm LEDs</t>
+  </si>
+  <si>
+    <t>IR Break Beam Sensor with Premium Wire Header Ends - 5mm LEDs : ID 2168 : Adafruit Industries, Unique &amp; fun DIY electronics and kits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,17 +178,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <charset val="1"/>
     </font>
     <font>
@@ -254,16 +226,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -525,18 +498,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.21875" customWidth="1"/>
     <col min="2" max="2" width="31.21875" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="3" max="3" width="113.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.6640625" customWidth="1"/>
     <col min="5" max="5" width="103.33203125" customWidth="1"/>
     <col min="6" max="6" width="43.109375" customWidth="1"/>
@@ -568,9 +541,9 @@
         <f>'Communication BOM'!B1</f>
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="str">
         <f>'Break Beam BOM'!B1</f>
-        <v>0</v>
+        <v>IR Break Beam Sensor with Premium Wire Header Ends - 5mm LEDs</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>'Encoder BOM'!B1</f>
@@ -597,9 +570,9 @@
         <f>'Communication BOM'!B2</f>
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="str">
         <f>'Break Beam BOM'!B2</f>
-        <v>0</v>
+        <v>IR Break Beam Sensor with Premium Wire Header Ends - 5mm LEDs : ID 2168 : Adafruit Industries, Unique &amp; fun DIY electronics and kits</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>'Encoder BOM'!B2</f>
@@ -622,9 +595,9 @@
         <f>'Communication BOM'!B3</f>
         <v>0</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="str">
         <f>'Break Beam BOM'!B3</f>
-        <v>0</v>
+        <v>(20*10*8)</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>'Encoder BOM'!B3</f>
@@ -649,7 +622,7 @@
       </c>
       <c r="C5" s="2">
         <f>'Break Beam BOM'!B4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2">
         <f>'Encoder BOM'!B4</f>
@@ -674,7 +647,7 @@
       </c>
       <c r="C6" s="2">
         <f>'Break Beam BOM'!B5</f>
-        <v>0</v>
+        <v>60.928000000000004</v>
       </c>
       <c r="D6" s="2">
         <f>'Encoder BOM'!B5</f>
@@ -699,7 +672,7 @@
       </c>
       <c r="C7" s="2">
         <f>'Break Beam BOM'!B6</f>
-        <v>0</v>
+        <v>60.928000000000004</v>
       </c>
       <c r="D7" s="2">
         <f>'Encoder BOM'!B6</f>
@@ -725,9 +698,9 @@
         <f>'Communication BOM'!D1</f>
         <v>0</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="4" t="str">
         <f>'Break Beam BOM'!D1</f>
-        <v>0</v>
+        <v>IR Break Beam Sensors with Premium Wire Header Ends - 3mm LEDs</v>
       </c>
       <c r="D9" s="4" t="str">
         <f>'Encoder BOM'!D1</f>
@@ -750,9 +723,9 @@
         <f>'Communication BOM'!D2</f>
         <v>0</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="4" t="str">
         <f>'Break Beam BOM'!D2</f>
-        <v>0</v>
+        <v>IR Break Beam Sensors with Premium Wire Header Ends - 3mm LEDs : ID 2167 : Adafruit Industries, Unique &amp; fun DIY electronics and kits</v>
       </c>
       <c r="D10" s="4" t="str">
         <f>'Encoder BOM'!D2</f>
@@ -775,9 +748,9 @@
         <f>'Communication BOM'!D3</f>
         <v>0</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="4" t="str">
         <f>'Break Beam BOM'!D3</f>
-        <v>0</v>
+        <v>(20*10*8)</v>
       </c>
       <c r="D11" s="4" t="str">
         <f>'Encoder BOM'!D3</f>
@@ -802,7 +775,7 @@
       </c>
       <c r="C12" s="4">
         <f>'Break Beam BOM'!D4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="4">
         <f>'Encoder BOM'!D4</f>
@@ -827,7 +800,7 @@
       </c>
       <c r="C13" s="4">
         <f>'Break Beam BOM'!D5</f>
-        <v>0</v>
+        <v>30.208000000000002</v>
       </c>
       <c r="D13" s="4">
         <f>'Encoder BOM'!D5</f>
@@ -852,7 +825,7 @@
       </c>
       <c r="C14" s="4">
         <f>'Break Beam BOM'!D6</f>
-        <v>0</v>
+        <v>30.208000000000002</v>
       </c>
       <c r="D14" s="4">
         <f>'Encoder BOM'!D6</f>
@@ -1023,7 +996,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1146,15 +1118,15 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="2" customWidth="1"/>
+    <col min="2" max="2" width="113.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="2" customWidth="1"/>
+    <col min="4" max="4" width="56.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
     <col min="6" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" customWidth="1"/>
@@ -1175,8 +1147,14 @@
       <c r="A1" t="s">
         <v>5</v>
       </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
       <c r="C1" t="s">
         <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
       </c>
       <c r="E1" t="s">
         <v>13</v>
@@ -1190,8 +1168,14 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="C2" t="s">
         <v>12</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1201,8 +1185,14 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
       <c r="C3" t="s">
         <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1212,8 +1202,14 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
       <c r="C4" t="s">
         <v>14</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -1223,8 +1219,16 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="B5">
+        <f>10.24*5.95</f>
+        <v>60.928000000000004</v>
+      </c>
       <c r="C5" t="s">
         <v>9</v>
+      </c>
+      <c r="D5">
+        <f>10.24*2.95</f>
+        <v>30.208000000000002</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -1234,12 +1238,16 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
+      <c r="B6">
+        <f>B4*B5</f>
+        <v>60.928000000000004</v>
+      </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6">
         <f>D4*D5</f>
-        <v>0</v>
+        <v>30.208000000000002</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1250,8 +1258,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://www.adafruit.com/product/2167" xr:uid="{57993EA2-747B-4AE5-807D-E363B2ABE16D}"/>
+    <hyperlink ref="B2" r:id="rId2" display="https://www.adafruit.com/product/2168" xr:uid="{A86CBDD0-4070-4ACB-913B-CBB24F3417FB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated the BOM lists with additional components.
</commit_message>
<xml_diff>
--- a/BOM/RoboCUP_SSL_Hardware_BOM.xlsx
+++ b/BOM/RoboCUP_SSL_Hardware_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fnl18001\OneDrive - Mälardalens universitet\Robotics_program_university\Ongoing_courses\DVA490\SSL-Hardware-Development\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/fnl18001_student_mdu_se/Documents/Robotics_program_university/Ongoing_courses/DVA490/SSL-Hardware-Development/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_746B6E28CE293E4F3E464F6686B02C4FF617E8F7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3CD2EEE0-48D2-4CF5-B9D2-A2FB5DC246C8}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="11_746B6E28CE293E4F3E464F6686B02C4FF617E8F7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F892E946-5C04-4380-9CF0-3976955E676D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete BOM" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="43">
   <si>
     <t>Communication Component</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>IR Break Beam Sensor with Premium Wire Header Ends - 5mm LEDs : ID 2168 : Adafruit Industries, Unique &amp; fun DIY electronics and kits</t>
+  </si>
+  <si>
+    <t>Officiell Raspberry Pi HQ-kamera 12,3 MP ned SONY IMX477R- sensor</t>
+  </si>
+  <si>
+    <t>r-pi</t>
+  </si>
+  <si>
+    <t>38*38*18,43)</t>
   </si>
 </sst>
 </file>
@@ -228,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -237,6 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +565,7 @@
       </c>
       <c r="F2" s="2" t="str">
         <f>'Obstical detection BOM'!B1</f>
-        <v>OPT8241NBN</v>
+        <v>Officiell Raspberry Pi HQ-kamera 12,3 MP ned SONY IMX477R- sensor</v>
       </c>
       <c r="R2">
         <f>P2*Q2</f>
@@ -584,7 +594,7 @@
       </c>
       <c r="F3" s="2" t="str">
         <f>'Obstical detection BOM'!B2</f>
-        <v>OPT8241NBN Texas Instruments | Mouser Sverige</v>
+        <v>r-pi</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -609,7 +619,7 @@
       </c>
       <c r="F4" s="2" t="str">
         <f>'Obstical detection BOM'!B3</f>
-        <v>7,9*8,8*0,8</v>
+        <v>38*38*18,43)</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -659,7 +669,7 @@
       </c>
       <c r="F6" s="2">
         <f>'Obstical detection BOM'!B5</f>
-        <v>605.13</v>
+        <v>698</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -684,7 +694,7 @@
       </c>
       <c r="F7" s="2">
         <f>'Obstical detection BOM'!B6</f>
-        <v>605.13</v>
+        <v>698</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -710,9 +720,9 @@
         <f>'IMU BOM'!D1</f>
         <v>0</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="4" t="str">
         <f>'Obstical detection BOM'!D1</f>
-        <v>0</v>
+        <v>OPT8241NBN</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -735,9 +745,9 @@
         <f>'IMU BOM'!D2</f>
         <v>0</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="4" t="str">
         <f>'Obstical detection BOM'!D2</f>
-        <v>0</v>
+        <v>OPT8241NBN Texas Instruments | Mouser Sverige</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -760,9 +770,9 @@
         <f>'IMU BOM'!D3</f>
         <v>0</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="4" t="str">
         <f>'Obstical detection BOM'!D3</f>
-        <v>0</v>
+        <v>7,9*8,8*0,8</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -787,7 +797,7 @@
       </c>
       <c r="F12" s="4">
         <f>'Obstical detection BOM'!D4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -812,7 +822,7 @@
       </c>
       <c r="F13" s="4">
         <f>'Obstical detection BOM'!D5</f>
-        <v>0</v>
+        <v>605.13</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -837,7 +847,7 @@
       </c>
       <c r="F14" s="4">
         <f>'Obstical detection BOM'!D6</f>
-        <v>0</v>
+        <v>605.13</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -1602,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1611,7 +1621,7 @@
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="2" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
     <col min="6" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" customWidth="1"/>
@@ -1633,10 +1643,13 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
       </c>
       <c r="E1" t="s">
         <v>13</v>
@@ -1650,11 +1663,14 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>33</v>
+      <c r="B2" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1665,10 +1681,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1684,6 +1703,9 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
@@ -1693,10 +1715,13 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>605.13</v>
+        <v>698</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
+      </c>
+      <c r="D5">
+        <v>605.13</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -1708,14 +1733,14 @@
       </c>
       <c r="B6">
         <f>B4*B5</f>
-        <v>605.13</v>
+        <v>698</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6">
         <f>D4*D5</f>
-        <v>0</v>
+        <v>605.13</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1727,7 +1752,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{E5B8FF7C-875F-4748-8F34-4C06611B4EC6}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{F90DF394-D00E-4A31-ABED-5A5470CD174D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Changed communication column since the ESP32 supports Wifi there is no need for additional communication hardware.
</commit_message>
<xml_diff>
--- a/BOM/RoboCUP_SSL_Hardware_BOM.xlsx
+++ b/BOM/RoboCUP_SSL_Hardware_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/fnl18001_student_mdu_se/Documents/Robotics_program_university/Ongoing_courses/DVA490/SSL-Hardware-Development/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_746B6E28CE293E4F3E464F6686B02C4FF617E8F7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F892E946-5C04-4380-9CF0-3976955E676D}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_746B6E28CE293E4F3E464F6686B02C4FF617E8F7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4F63CB6A-2F83-4BBF-AA30-C96559F409E7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete BOM" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="44">
   <si>
     <t>Communication Component</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>38*38*18,43)</t>
+  </si>
+  <si>
+    <t>Not applicable since ESP32 supports WiFi communication</t>
   </si>
 </sst>
 </file>
@@ -511,18 +514,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.21875" customWidth="1"/>
-    <col min="2" max="2" width="31.21875" customWidth="1"/>
+    <col min="2" max="2" width="48.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="113.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.6640625" customWidth="1"/>
     <col min="5" max="5" width="103.33203125" customWidth="1"/>
-    <col min="6" max="6" width="43.109375" customWidth="1"/>
+    <col min="6" max="6" width="58.5546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -547,9 +550,9 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="2" t="str">
         <f>'Communication BOM'!B1</f>
-        <v>0</v>
+        <v>Not applicable since ESP32 supports WiFi communication</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>'Break Beam BOM'!B1</f>
@@ -1014,15 +1017,15 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="48.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
     <col min="6" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" customWidth="1"/>
@@ -1042,6 +1045,9 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
@@ -1612,7 +1618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added a few comments and addtional hardware to the BOM. After speaking with Emil it was suggested that it would be beneficial to make sure that the camera and the microcontroller support each other.
</commit_message>
<xml_diff>
--- a/BOM/RoboCUP_SSL_Hardware_BOM.xlsx
+++ b/BOM/RoboCUP_SSL_Hardware_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/fnl18001_student_mdu_se/Documents/Robotics_program_university/Ongoing_courses/DVA490/SSL-Hardware-Development/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="11_746B6E28CE293E4F3E464F6686B02C4FF617E8F7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4F63CB6A-2F83-4BBF-AA30-C96559F409E7}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="11_746B6E28CE293E4F3E464F6686B02C4FF617E8F7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{737BFB06-C4ED-4CC2-A4E8-0475E1053C90}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,8 +29,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Fredrik Westerbom</author>
+  </authors>
+  <commentList>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{CAE2C77D-A078-45A2-A933-39814B1EC7E8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fredrik Westerbom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Please see the 'Obsticle detection BOM' sheet for additional information.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="48">
   <si>
     <t>Communication Component</t>
   </si>
@@ -119,9 +153,6 @@
     <t>WSEN-ISDS 6 Axis IMU</t>
   </si>
   <si>
-    <t>⁣WSEN-ISDS 6 Axis IMU (Inertial Measurement Unit) &amp; EV-Kits | Sensors | Würth Elektronik Product Catalog (we-online.com)</t>
-  </si>
-  <si>
     <t>3,0*2,5*0,86</t>
   </si>
   <si>
@@ -140,18 +171,12 @@
     <t>IR Break Beam Sensors with Premium Wire Header Ends - 3mm LEDs</t>
   </si>
   <si>
-    <t>IR Break Beam Sensors with Premium Wire Header Ends - 3mm LEDs : ID 2167 : Adafruit Industries, Unique &amp; fun DIY electronics and kits</t>
-  </si>
-  <si>
     <t>(20*10*8)</t>
   </si>
   <si>
     <t>IR Break Beam Sensor with Premium Wire Header Ends - 5mm LEDs</t>
   </si>
   <si>
-    <t>IR Break Beam Sensor with Premium Wire Header Ends - 5mm LEDs : ID 2168 : Adafruit Industries, Unique &amp; fun DIY electronics and kits</t>
-  </si>
-  <si>
     <t>Officiell Raspberry Pi HQ-kamera 12,3 MP ned SONY IMX477R- sensor</t>
   </si>
   <si>
@@ -162,13 +187,34 @@
   </si>
   <si>
     <t>Not applicable since ESP32 supports WiFi communication</t>
+  </si>
+  <si>
+    <t>Adafruit 5mm</t>
+  </si>
+  <si>
+    <t>Adafruit 3mm</t>
+  </si>
+  <si>
+    <t>we-online</t>
+  </si>
+  <si>
+    <t>Additional Component</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 3 Model A+</t>
+  </si>
+  <si>
+    <t>Electro:kit Raspberry Pi 3</t>
+  </si>
+  <si>
+    <t>(65*56*10)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +244,19 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -334,6 +393,76 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7970580" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FEFA8FE-2683-4487-A180-1191908A75FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30480" y="1790700"/>
+          <a:ext cx="7970580" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100"/>
+            <a:t>If we are going with our</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100" baseline="0"/>
+            <a:t> primary component we will need Raspberry Pi as well. Please see the additional component specification below</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="sv-SE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -511,11 +640,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,7 +714,7 @@
       </c>
       <c r="C3" s="2" t="str">
         <f>'Break Beam BOM'!B2</f>
-        <v>IR Break Beam Sensor with Premium Wire Header Ends - 5mm LEDs : ID 2168 : Adafruit Industries, Unique &amp; fun DIY electronics and kits</v>
+        <v>Adafruit 5mm</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>'Encoder BOM'!B2</f>
@@ -593,7 +722,7 @@
       </c>
       <c r="E3" s="2" t="str">
         <f>'IMU BOM'!B2</f>
-        <v>⁣WSEN-ISDS 6 Axis IMU (Inertial Measurement Unit) &amp; EV-Kits | Sensors | Würth Elektronik Product Catalog (we-online.com)</v>
+        <v>we-online</v>
       </c>
       <c r="F3" s="2" t="str">
         <f>'Obstical detection BOM'!B2</f>
@@ -738,7 +867,7 @@
       </c>
       <c r="C10" s="4" t="str">
         <f>'Break Beam BOM'!D2</f>
-        <v>IR Break Beam Sensors with Premium Wire Header Ends - 3mm LEDs : ID 2167 : Adafruit Industries, Unique &amp; fun DIY electronics and kits</v>
+        <v>Adafruit 3mm</v>
       </c>
       <c r="D10" s="4" t="str">
         <f>'Encoder BOM'!D2</f>
@@ -1009,6 +1138,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1047,7 +1177,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
@@ -1134,7 +1264,7 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,13 +1294,13 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
         <v>13</v>
@@ -1185,13 +1315,13 @@
         <v>12</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1202,13 +1332,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1275,8 +1405,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://www.adafruit.com/product/2167" xr:uid="{57993EA2-747B-4AE5-807D-E363B2ABE16D}"/>
-    <hyperlink ref="B2" r:id="rId2" display="https://www.adafruit.com/product/2168" xr:uid="{A86CBDD0-4070-4ACB-913B-CBB24F3417FB}"/>
+    <hyperlink ref="B2" r:id="rId1" display="Adafruit" xr:uid="{FEFDF3C0-111B-4E9D-99F0-4B4C5211F93A}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{C13F210E-370F-4FB1-AD06-6465D677BD3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -1483,7 +1613,7 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1530,8 +1660,8 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>29</v>
+      <c r="B2" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -1545,7 +1675,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -1573,7 +1703,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -1607,7 +1737,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="2536030320001" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" location="2536030320001" xr:uid="{E7FB9528-54D0-4589-A2BE-5123F733AF4F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1616,10 +1746,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1649,13 +1779,13 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
         <v>13</v>
@@ -1670,13 +1800,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1687,13 +1817,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1754,14 +1884,65 @@
       <c r="F6">
         <f>F4*F5</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <f>B16*B17</f>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{E5B8FF7C-875F-4748-8F34-4C06611B4EC6}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{F90DF394-D00E-4A31-ABED-5A5470CD174D}"/>
+    <hyperlink ref="B14" r:id="rId3" xr:uid="{C4091ABB-FB3F-4D6C-999E-2A7FEC7CC0AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished the BOM for communication and sensors. Added the last obsticle detection sensor, an ESP32-CAM which includes a camera as well as a development board.
</commit_message>
<xml_diff>
--- a/BOM/RoboCUP_SSL_Hardware_BOM.xlsx
+++ b/BOM/RoboCUP_SSL_Hardware_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/fnl18001_student_mdu_se/Documents/Robotics_program_university/Ongoing_courses/DVA490/SSL-Hardware-Development/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="11_746B6E28CE293E4F3E464F6686B02C4FF617E8F7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{737BFB06-C4ED-4CC2-A4E8-0475E1053C90}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="11_746B6E28CE293E4F3E464F6686B02C4FF617E8F7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{CEE15753-AED5-4A11-B5DD-AE0D27337307}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="51">
   <si>
     <t>Communication Component</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>(65*56*10)</t>
+  </si>
+  <si>
+    <t>ESP32-CAM Utvecklingskort</t>
+  </si>
+  <si>
+    <t>Electro:kit - ESP32 url</t>
+  </si>
+  <si>
+    <t>(40*27*15)</t>
   </si>
 </sst>
 </file>
@@ -644,7 +653,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,9 +842,7 @@
       <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="B9" s="4">
         <f>'Communication BOM'!D1</f>
         <v>0</v>
@@ -854,7 +861,7 @@
       </c>
       <c r="F9" s="4" t="str">
         <f>'Obstical detection BOM'!D1</f>
-        <v>OPT8241NBN</v>
+        <v>ESP32-CAM Utvecklingskort</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -879,7 +886,7 @@
       </c>
       <c r="F10" s="4" t="str">
         <f>'Obstical detection BOM'!D2</f>
-        <v>OPT8241NBN Texas Instruments | Mouser Sverige</v>
+        <v>Electro:kit - ESP32 url</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -904,7 +911,7 @@
       </c>
       <c r="F11" s="4" t="str">
         <f>'Obstical detection BOM'!D3</f>
-        <v>7,9*8,8*0,8</v>
+        <v>(40*27*15)</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -954,7 +961,7 @@
       </c>
       <c r="F13" s="4">
         <f>'Obstical detection BOM'!D5</f>
-        <v>605.13</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -979,7 +986,7 @@
       </c>
       <c r="F14" s="4">
         <f>'Obstical detection BOM'!D6</f>
-        <v>605.13</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -1005,9 +1012,9 @@
         <f>'IMU BOM'!F1</f>
         <v>0</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="5" t="str">
         <f>'Obstical detection BOM'!F1</f>
-        <v>0</v>
+        <v>OPT8241NBN</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1030,9 +1037,9 @@
         <f>'IMU BOM'!F2</f>
         <v>0</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="5" t="str">
         <f>'Obstical detection BOM'!F2</f>
-        <v>0</v>
+        <v>OPT8241NBN Texas Instruments | Mouser Sverige</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1055,9 +1062,9 @@
         <f>'IMU BOM'!F3</f>
         <v>0</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="5" t="str">
         <f>'Obstical detection BOM'!F3</f>
-        <v>0</v>
+        <v>7,9*8,8*0,8</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1082,7 +1089,7 @@
       </c>
       <c r="F19" s="5">
         <f>'Obstical detection BOM'!F4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1107,7 +1114,7 @@
       </c>
       <c r="F20" s="5">
         <f>'Obstical detection BOM'!F5</f>
-        <v>0</v>
+        <v>605.13</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1132,7 +1139,7 @@
       </c>
       <c r="F21" s="5">
         <f>'Obstical detection BOM'!F6</f>
-        <v>0</v>
+        <v>605.13</v>
       </c>
     </row>
   </sheetData>
@@ -1749,17 +1756,17 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="2" max="2" width="58.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" customWidth="1"/>
     <col min="4" max="4" width="42.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="2" customWidth="1"/>
+    <col min="6" max="6" width="42.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" customWidth="1"/>
     <col min="8" max="8" width="9.77734375" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
@@ -1785,10 +1792,13 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
         <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
       </c>
       <c r="R1">
         <f>P1*Q1</f>
@@ -1805,11 +1815,14 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>32</v>
+      <c r="D2" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -1823,10 +1836,13 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -1845,6 +1861,9 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1857,10 +1876,13 @@
         <v>9</v>
       </c>
       <c r="D5">
-        <v>605.13</v>
+        <v>199</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
+      </c>
+      <c r="F5">
+        <v>605.13</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -1876,14 +1898,14 @@
       </c>
       <c r="D6">
         <f>D4*D5</f>
-        <v>605.13</v>
+        <v>199</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6">
         <f>F4*F5</f>
-        <v>0</v>
+        <v>605.13</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -1937,12 +1959,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{E5B8FF7C-875F-4748-8F34-4C06611B4EC6}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{E5B8FF7C-875F-4748-8F34-4C06611B4EC6}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{F90DF394-D00E-4A31-ABED-5A5470CD174D}"/>
     <hyperlink ref="B14" r:id="rId3" xr:uid="{C4091ABB-FB3F-4D6C-999E-2A7FEC7CC0AA}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{FA8BC5CD-CEC1-404C-8689-5B663593DB51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>